<commit_message>
First complete successful run through of the manuscript file after code restructure!
</commit_message>
<xml_diff>
--- a/manuscript/testsave.xlsx
+++ b/manuscript/testsave.xlsx
@@ -1759,58 +1759,58 @@
   <sheetData>
     <row r="1" spans="1:28">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>18</v>
@@ -1844,59 +1844,59 @@
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>48.2492073388727</v>
+      </c>
+      <c r="C2">
+        <v>2.22211385404349</v>
+      </c>
+      <c r="D2">
+        <v>11.6921940392032</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.0799988314202061</v>
+      </c>
+      <c r="I2">
+        <v>14.1838165358568</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>9.89273186356637</v>
+      </c>
+      <c r="M2">
+        <v>1.81052154253552</v>
+      </c>
+      <c r="N2">
+        <v>0.352013654046987</v>
+      </c>
+      <c r="O2">
+        <v>0.210479390362178</v>
+      </c>
+      <c r="P2">
+        <v>0.4246947187776288</v>
+      </c>
+      <c r="Q2">
+        <v>0.002873020370883501</v>
+      </c>
+      <c r="R2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
+      <c r="S2" t="s">
         <v>43</v>
-      </c>
-      <c r="D2">
-        <v>48.2492073388727</v>
-      </c>
-      <c r="E2">
-        <v>2.22211385404349</v>
-      </c>
-      <c r="F2">
-        <v>11.6921940392032</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0.0799988314202061</v>
-      </c>
-      <c r="K2">
-        <v>14.1838165358568</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>9.89273186356637</v>
-      </c>
-      <c r="O2">
-        <v>1.81052154253552</v>
-      </c>
-      <c r="P2">
-        <v>0.352013654046987</v>
-      </c>
-      <c r="Q2">
-        <v>0.210479390362178</v>
-      </c>
-      <c r="R2">
-        <v>0.4246947187776288</v>
-      </c>
-      <c r="S2">
-        <v>0.002873020370883501</v>
       </c>
       <c r="T2">
         <v>62.5</v>
@@ -1927,59 +1927,59 @@
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>48.2956914301173</v>
+      </c>
+      <c r="C3">
+        <v>2.16535749123189</v>
+      </c>
+      <c r="D3">
+        <v>11.7555842002198</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0.08404493440252241</v>
+      </c>
+      <c r="I3">
+        <v>13.403979652898</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>10.0525777926129</v>
+      </c>
+      <c r="M3">
+        <v>2.26819812005229</v>
+      </c>
+      <c r="N3">
+        <v>0.373327784000187</v>
+      </c>
+      <c r="O3">
+        <v>0.204452497579727</v>
+      </c>
+      <c r="P3">
+        <v>0.4259837834222454</v>
+      </c>
+      <c r="Q3">
+        <v>0.006786430337147899</v>
+      </c>
+      <c r="R3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" t="s">
+      <c r="S3" t="s">
         <v>43</v>
-      </c>
-      <c r="D3">
-        <v>48.2956914301173</v>
-      </c>
-      <c r="E3">
-        <v>2.16535749123189</v>
-      </c>
-      <c r="F3">
-        <v>11.7555842002198</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0.08404493440252241</v>
-      </c>
-      <c r="K3">
-        <v>13.403979652898</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>10.0525777926129</v>
-      </c>
-      <c r="O3">
-        <v>2.26819812005229</v>
-      </c>
-      <c r="P3">
-        <v>0.373327784000187</v>
-      </c>
-      <c r="Q3">
-        <v>0.204452497579727</v>
-      </c>
-      <c r="R3">
-        <v>0.4259837834222454</v>
-      </c>
-      <c r="S3">
-        <v>0.006786430337147899</v>
       </c>
       <c r="T3">
         <v>128</v>
@@ -2010,59 +2010,59 @@
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>49.1240791972564</v>
+      </c>
+      <c r="C4">
+        <v>2.36098425857992</v>
+      </c>
+      <c r="D4">
+        <v>12.1728325512416</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0.0988087330759878</v>
+      </c>
+      <c r="I4">
+        <v>11.997699453588</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>10.3081877392399</v>
+      </c>
+      <c r="M4">
+        <v>2.00186324677907</v>
+      </c>
+      <c r="N4">
+        <v>0.396511854205657</v>
+      </c>
+      <c r="O4">
+        <v>0.238996316060337</v>
+      </c>
+      <c r="P4">
+        <v>0.4377576296337298</v>
+      </c>
+      <c r="Q4">
+        <v>0.004983721604329198</v>
+      </c>
+      <c r="R4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" t="s">
+      <c r="S4" t="s">
         <v>43</v>
-      </c>
-      <c r="D4">
-        <v>49.1240791972564</v>
-      </c>
-      <c r="E4">
-        <v>2.36098425857992</v>
-      </c>
-      <c r="F4">
-        <v>12.1728325512416</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0.0988087330759878</v>
-      </c>
-      <c r="K4">
-        <v>11.997699453588</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>10.3081877392399</v>
-      </c>
-      <c r="O4">
-        <v>2.00186324677907</v>
-      </c>
-      <c r="P4">
-        <v>0.396511854205657</v>
-      </c>
-      <c r="Q4">
-        <v>0.238996316060337</v>
-      </c>
-      <c r="R4">
-        <v>0.4377576296337298</v>
-      </c>
-      <c r="S4">
-        <v>0.004983721604329198</v>
       </c>
       <c r="T4">
         <v>100</v>
@@ -2093,59 +2093,59 @@
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>47.96</v>
+      </c>
+      <c r="C5">
+        <v>0.78</v>
+      </c>
+      <c r="D5">
+        <v>18.77</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>10.92</v>
+      </c>
+      <c r="H5">
+        <v>0.15</v>
+      </c>
+      <c r="I5">
+        <v>6.86</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>12.23</v>
+      </c>
+      <c r="M5">
+        <v>1.95</v>
+      </c>
+      <c r="N5">
+        <v>0.21</v>
+      </c>
+      <c r="O5">
+        <v>0.17</v>
+      </c>
+      <c r="P5">
+        <v>4.5</v>
+      </c>
+      <c r="Q5">
+        <v>0.0479</v>
+      </c>
+      <c r="R5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" t="s">
+      <c r="S5" t="s">
         <v>43</v>
-      </c>
-      <c r="D5">
-        <v>47.96</v>
-      </c>
-      <c r="E5">
-        <v>0.78</v>
-      </c>
-      <c r="F5">
-        <v>18.77</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>10.92</v>
-      </c>
-      <c r="J5">
-        <v>0.15</v>
-      </c>
-      <c r="K5">
-        <v>6.86</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>12.23</v>
-      </c>
-      <c r="O5">
-        <v>1.95</v>
-      </c>
-      <c r="P5">
-        <v>0.21</v>
-      </c>
-      <c r="Q5">
-        <v>0.17</v>
-      </c>
-      <c r="R5">
-        <v>4.5</v>
-      </c>
-      <c r="S5">
-        <v>0.0479</v>
       </c>
       <c r="T5">
         <v>2000</v>
@@ -2176,59 +2176,59 @@
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>49.64</v>
+      </c>
+      <c r="C6">
+        <v>0.71</v>
+      </c>
+      <c r="D6">
+        <v>18.05</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>10.54</v>
+      </c>
+      <c r="H6">
+        <v>0.19</v>
+      </c>
+      <c r="I6">
+        <v>6.43</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>12.09</v>
+      </c>
+      <c r="M6">
+        <v>1.99</v>
+      </c>
+      <c r="N6">
+        <v>0.2</v>
+      </c>
+      <c r="O6">
+        <v>0.17</v>
+      </c>
+      <c r="P6">
+        <v>5.1</v>
+      </c>
+      <c r="Q6">
+        <v>0.1113</v>
+      </c>
+      <c r="R6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" t="s">
+      <c r="S6" t="s">
         <v>43</v>
-      </c>
-      <c r="D6">
-        <v>49.64</v>
-      </c>
-      <c r="E6">
-        <v>0.71</v>
-      </c>
-      <c r="F6">
-        <v>18.05</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>10.54</v>
-      </c>
-      <c r="J6">
-        <v>0.19</v>
-      </c>
-      <c r="K6">
-        <v>6.43</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>12.09</v>
-      </c>
-      <c r="O6">
-        <v>1.99</v>
-      </c>
-      <c r="P6">
-        <v>0.2</v>
-      </c>
-      <c r="Q6">
-        <v>0.17</v>
-      </c>
-      <c r="R6">
-        <v>5.1</v>
-      </c>
-      <c r="S6">
-        <v>0.1113</v>
       </c>
       <c r="T6">
         <v>2000</v>
@@ -2259,59 +2259,59 @@
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>50.32</v>
+      </c>
+      <c r="C7">
+        <v>0.72</v>
+      </c>
+      <c r="D7">
+        <v>18.03</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>10.11</v>
+      </c>
+      <c r="H7">
+        <v>0.14</v>
+      </c>
+      <c r="I7">
+        <v>5.65</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>12.78</v>
+      </c>
+      <c r="M7">
+        <v>1.8</v>
+      </c>
+      <c r="N7">
+        <v>0.24</v>
+      </c>
+      <c r="O7">
+        <v>0.23</v>
+      </c>
+      <c r="P7">
+        <v>5.2</v>
+      </c>
+      <c r="Q7">
+        <v>0.0437</v>
+      </c>
+      <c r="R7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
+      <c r="S7" t="s">
         <v>43</v>
-      </c>
-      <c r="D7">
-        <v>50.32</v>
-      </c>
-      <c r="E7">
-        <v>0.72</v>
-      </c>
-      <c r="F7">
-        <v>18.03</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>10.11</v>
-      </c>
-      <c r="J7">
-        <v>0.14</v>
-      </c>
-      <c r="K7">
-        <v>5.65</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>12.78</v>
-      </c>
-      <c r="O7">
-        <v>1.8</v>
-      </c>
-      <c r="P7">
-        <v>0.24</v>
-      </c>
-      <c r="Q7">
-        <v>0.23</v>
-      </c>
-      <c r="R7">
-        <v>5.2</v>
-      </c>
-      <c r="S7">
-        <v>0.0437</v>
       </c>
       <c r="T7">
         <v>2000</v>
@@ -2342,59 +2342,59 @@
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
+      <c r="B8">
+        <v>62.6</v>
+      </c>
+      <c r="C8">
+        <v>0.63</v>
       </c>
       <c r="D8">
-        <v>62.6</v>
+        <v>17.3</v>
       </c>
       <c r="E8">
-        <v>0.63</v>
+        <v>2.01</v>
       </c>
       <c r="F8">
-        <v>17.3</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>2.01</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="I8">
-        <v>2.01</v>
+        <v>2.65</v>
       </c>
       <c r="J8">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>2.65</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>5.64</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>4.05</v>
       </c>
       <c r="N8">
-        <v>5.64</v>
+        <v>1.61</v>
       </c>
       <c r="O8">
-        <v>4.05</v>
+        <v>0.24</v>
       </c>
       <c r="P8">
-        <v>1.61</v>
+        <v>2.62</v>
       </c>
       <c r="Q8">
-        <v>0.24</v>
-      </c>
-      <c r="R8">
-        <v>2.62</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="R8" t="s">
+        <v>39</v>
+      </c>
+      <c r="S8" t="s">
+        <v>44</v>
       </c>
       <c r="T8">
         <v>703</v>
@@ -2425,59 +2425,59 @@
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>44</v>
+      <c r="B9">
+        <v>62.6</v>
+      </c>
+      <c r="C9">
+        <v>0.63</v>
       </c>
       <c r="D9">
-        <v>62.6</v>
+        <v>17.3</v>
       </c>
       <c r="E9">
-        <v>0.63</v>
+        <v>2.01</v>
       </c>
       <c r="F9">
-        <v>17.3</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>2.01</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="I9">
-        <v>2.01</v>
+        <v>2.65</v>
       </c>
       <c r="J9">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>2.65</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>5.64</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>4.05</v>
       </c>
       <c r="N9">
-        <v>5.64</v>
+        <v>1.61</v>
       </c>
       <c r="O9">
-        <v>4.05</v>
+        <v>0.24</v>
       </c>
       <c r="P9">
-        <v>1.61</v>
+        <v>5.03</v>
       </c>
       <c r="Q9">
-        <v>0.24</v>
-      </c>
-      <c r="R9">
-        <v>5.03</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="R9" t="s">
+        <v>39</v>
+      </c>
+      <c r="S9" t="s">
+        <v>44</v>
       </c>
       <c r="T9">
         <v>1865</v>
@@ -2508,59 +2508,59 @@
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
+      <c r="B10">
+        <v>62.6</v>
+      </c>
+      <c r="C10">
+        <v>0.63</v>
       </c>
       <c r="D10">
-        <v>62.6</v>
+        <v>17.3</v>
       </c>
       <c r="E10">
-        <v>0.63</v>
+        <v>2.01</v>
       </c>
       <c r="F10">
-        <v>17.3</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>2.01</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="I10">
-        <v>2.01</v>
+        <v>2.65</v>
       </c>
       <c r="J10">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>2.65</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>5.64</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>4.05</v>
       </c>
       <c r="N10">
-        <v>5.64</v>
+        <v>1.61</v>
       </c>
       <c r="O10">
-        <v>4.05</v>
+        <v>0.24</v>
       </c>
       <c r="P10">
-        <v>1.61</v>
+        <v>6.76</v>
       </c>
       <c r="Q10">
-        <v>0.24</v>
-      </c>
-      <c r="R10">
-        <v>6.76</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="R10" t="s">
+        <v>39</v>
+      </c>
+      <c r="S10" t="s">
+        <v>44</v>
       </c>
       <c r="T10">
         <v>2985</v>
@@ -2591,59 +2591,59 @@
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11">
+        <v>76.9748797434527</v>
+      </c>
+      <c r="C11">
+        <v>0.085515766969535</v>
+      </c>
+      <c r="D11">
+        <v>3.11063602351684</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>4.78888295029396</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>12.5494388027793</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>1.20791020844468</v>
+      </c>
+      <c r="M11">
+        <v>0.138963121325494</v>
+      </c>
+      <c r="N11">
+        <v>1.13308391234634</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>4.34</v>
+      </c>
+      <c r="Q11">
+        <v>0.007</v>
+      </c>
+      <c r="R11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
+      <c r="S11" t="s">
         <v>45</v>
-      </c>
-      <c r="D11">
-        <v>76.9748797434527</v>
-      </c>
-      <c r="E11">
-        <v>0.085515766969535</v>
-      </c>
-      <c r="F11">
-        <v>3.11063602351684</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>4.78888295029396</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>12.5494388027793</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>1.20791020844468</v>
-      </c>
-      <c r="O11">
-        <v>0.138963121325494</v>
-      </c>
-      <c r="P11">
-        <v>1.13308391234634</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>4.34</v>
-      </c>
-      <c r="S11">
-        <v>0.007</v>
       </c>
       <c r="T11">
         <v>300</v>
@@ -2674,59 +2674,59 @@
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12">
+        <v>76.9438448701072</v>
+      </c>
+      <c r="C12">
+        <v>0.133124692583271</v>
+      </c>
+      <c r="D12">
+        <v>3.16965680268094</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>4.76343532834393</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>12.4464028247851</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>1.23172756929903</v>
+      </c>
+      <c r="M12">
+        <v>0.140993377177016</v>
+      </c>
+      <c r="N12">
+        <v>1.17080646457768</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>5.85</v>
+      </c>
+      <c r="Q12">
+        <v>0.0123</v>
+      </c>
+      <c r="R12" t="s">
         <v>40</v>
       </c>
-      <c r="C12" t="s">
+      <c r="S12" t="s">
         <v>45</v>
-      </c>
-      <c r="D12">
-        <v>76.9438448701072</v>
-      </c>
-      <c r="E12">
-        <v>0.133124692583271</v>
-      </c>
-      <c r="F12">
-        <v>3.16965680268094</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>4.76343532834393</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>12.4464028247851</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>1.23172756929903</v>
-      </c>
-      <c r="O12">
-        <v>0.140993377177016</v>
-      </c>
-      <c r="P12">
-        <v>1.17080646457768</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>5.85</v>
-      </c>
-      <c r="S12">
-        <v>0.0123</v>
       </c>
       <c r="T12">
         <v>300</v>
@@ -2757,59 +2757,59 @@
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13">
+        <v>77.18720482277639</v>
+      </c>
+      <c r="C13">
+        <v>0.119505939828248</v>
+      </c>
+      <c r="D13">
+        <v>3.16782734403283</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>4.81407626970865</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>12.2295344248926</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>1.1847733013638</v>
+      </c>
+      <c r="M13">
+        <v>0.138201136168266</v>
+      </c>
+      <c r="N13">
+        <v>1.15892356512203</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>5.7545705764358</v>
+      </c>
+      <c r="Q13">
+        <v>0.0106631828985553</v>
+      </c>
+      <c r="R13" t="s">
         <v>40</v>
       </c>
-      <c r="C13" t="s">
+      <c r="S13" t="s">
         <v>45</v>
-      </c>
-      <c r="D13">
-        <v>77.18720482277639</v>
-      </c>
-      <c r="E13">
-        <v>0.119505939828248</v>
-      </c>
-      <c r="F13">
-        <v>3.16782734403283</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>4.81407626970865</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>12.2295344248926</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>1.1847733013638</v>
-      </c>
-      <c r="O13">
-        <v>0.138201136168266</v>
-      </c>
-      <c r="P13">
-        <v>1.15892356512203</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>5.7545705764358</v>
-      </c>
-      <c r="S13">
-        <v>0.0106631828985553</v>
       </c>
       <c r="T13">
         <v>300</v>
@@ -2840,59 +2840,59 @@
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14">
+        <v>75.4139659380119</v>
+      </c>
+      <c r="C14">
+        <v>0.09516411818348949</v>
+      </c>
+      <c r="D14">
+        <v>14.0776920173468</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0.654991693057126</v>
+      </c>
+      <c r="H14">
+        <v>0.125882451591361</v>
+      </c>
+      <c r="I14">
+        <v>0.0120034926222446</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0.636123687792963</v>
+      </c>
+      <c r="M14">
+        <v>3.70311026077796</v>
+      </c>
+      <c r="N14">
+        <v>5.12839160076096</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>5.94375</v>
+      </c>
+      <c r="Q14">
+        <v>0.01</v>
+      </c>
+      <c r="R14" t="s">
         <v>41</v>
       </c>
-      <c r="C14" t="s">
+      <c r="S14" t="s">
         <v>45</v>
-      </c>
-      <c r="D14">
-        <v>75.4139659380119</v>
-      </c>
-      <c r="E14">
-        <v>0.09516411818348949</v>
-      </c>
-      <c r="F14">
-        <v>14.0776920173468</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0.654991693057126</v>
-      </c>
-      <c r="J14">
-        <v>0.125882451591361</v>
-      </c>
-      <c r="K14">
-        <v>0.0120034926222446</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0.636123687792963</v>
-      </c>
-      <c r="O14">
-        <v>3.70311026077796</v>
-      </c>
-      <c r="P14">
-        <v>5.12839160076096</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>5.94375</v>
-      </c>
-      <c r="S14">
-        <v>0.01</v>
       </c>
       <c r="T14">
         <v>300</v>
@@ -2923,59 +2923,59 @@
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15">
+        <v>76.61358570474</v>
+      </c>
+      <c r="C15">
+        <v>0.0958432095376958</v>
+      </c>
+      <c r="D15">
+        <v>13.4767620639456</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0.620768528609716</v>
+      </c>
+      <c r="H15">
+        <v>0.113495070210069</v>
+      </c>
+      <c r="I15">
+        <v>0.0320690056690404</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0.624350060794128</v>
+      </c>
+      <c r="M15">
+        <v>3.6769719537635</v>
+      </c>
+      <c r="N15">
+        <v>4.57979937724531</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>5.34</v>
+      </c>
+      <c r="Q15">
+        <v>0.008</v>
+      </c>
+      <c r="R15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" t="s">
+      <c r="S15" t="s">
         <v>45</v>
-      </c>
-      <c r="D15">
-        <v>76.61358570474</v>
-      </c>
-      <c r="E15">
-        <v>0.0958432095376958</v>
-      </c>
-      <c r="F15">
-        <v>13.4767620639456</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0.620768528609716</v>
-      </c>
-      <c r="J15">
-        <v>0.113495070210069</v>
-      </c>
-      <c r="K15">
-        <v>0.0320690056690404</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0.624350060794128</v>
-      </c>
-      <c r="O15">
-        <v>3.6769719537635</v>
-      </c>
-      <c r="P15">
-        <v>4.57979937724531</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>5.34</v>
-      </c>
-      <c r="S15">
-        <v>0.008</v>
       </c>
       <c r="T15">
         <v>0</v>
@@ -3006,59 +3006,59 @@
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16">
+        <v>48.03</v>
+      </c>
+      <c r="C16">
+        <v>2.84</v>
+      </c>
+      <c r="D16">
+        <v>18.12</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>9.6</v>
+      </c>
+      <c r="H16">
+        <v>0.23</v>
+      </c>
+      <c r="I16">
+        <v>3.08</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>7.57</v>
+      </c>
+      <c r="M16">
+        <v>6.04</v>
+      </c>
+      <c r="N16">
+        <v>3.08</v>
+      </c>
+      <c r="O16">
+        <v>1.41</v>
+      </c>
+      <c r="P16">
+        <v>1.42</v>
+      </c>
+      <c r="Q16">
+        <v>0.1298</v>
+      </c>
+      <c r="R16" t="s">
         <v>42</v>
       </c>
-      <c r="C16" t="s">
+      <c r="S16" t="s">
         <v>46</v>
-      </c>
-      <c r="D16">
-        <v>48.03</v>
-      </c>
-      <c r="E16">
-        <v>2.84</v>
-      </c>
-      <c r="F16">
-        <v>18.12</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>9.6</v>
-      </c>
-      <c r="J16">
-        <v>0.23</v>
-      </c>
-      <c r="K16">
-        <v>3.08</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>7.57</v>
-      </c>
-      <c r="O16">
-        <v>6.04</v>
-      </c>
-      <c r="P16">
-        <v>3.08</v>
-      </c>
-      <c r="Q16">
-        <v>1.41</v>
-      </c>
-      <c r="R16">
-        <v>1.42</v>
-      </c>
-      <c r="S16">
-        <v>0.1298</v>
       </c>
       <c r="T16">
         <v>1500</v>
@@ -3089,59 +3089,59 @@
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17">
+        <v>52.98</v>
+      </c>
+      <c r="C17">
+        <v>2.18</v>
+      </c>
+      <c r="D17">
+        <v>20.49</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>5.54</v>
+      </c>
+      <c r="H17">
+        <v>0.2</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>7.1</v>
+      </c>
+      <c r="M17">
+        <v>5.68</v>
+      </c>
+      <c r="N17">
+        <v>3.16</v>
+      </c>
+      <c r="O17">
+        <v>0.66</v>
+      </c>
+      <c r="P17">
+        <v>4.76</v>
+      </c>
+      <c r="Q17">
+        <v>0.3439</v>
+      </c>
+      <c r="R17" t="s">
         <v>42</v>
       </c>
-      <c r="C17" t="s">
+      <c r="S17" t="s">
         <v>47</v>
-      </c>
-      <c r="D17">
-        <v>52.98</v>
-      </c>
-      <c r="E17">
-        <v>2.18</v>
-      </c>
-      <c r="F17">
-        <v>20.49</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>5.54</v>
-      </c>
-      <c r="J17">
-        <v>0.2</v>
-      </c>
-      <c r="K17">
-        <v>2</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>7.1</v>
-      </c>
-      <c r="O17">
-        <v>5.68</v>
-      </c>
-      <c r="P17">
-        <v>3.16</v>
-      </c>
-      <c r="Q17">
-        <v>0.66</v>
-      </c>
-      <c r="R17">
-        <v>4.76</v>
-      </c>
-      <c r="S17">
-        <v>0.3439</v>
       </c>
       <c r="T17">
         <v>4000</v>
@@ -3172,59 +3172,59 @@
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18">
+        <v>44.61</v>
+      </c>
+      <c r="C18">
+        <v>4.37</v>
+      </c>
+      <c r="D18">
+        <v>14.41</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>10.6</v>
+      </c>
+      <c r="H18">
+        <v>0.17</v>
+      </c>
+      <c r="I18">
+        <v>7.69</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>11.55</v>
+      </c>
+      <c r="M18">
+        <v>3.93</v>
+      </c>
+      <c r="N18">
+        <v>1.74</v>
+      </c>
+      <c r="O18">
+        <v>0.92</v>
+      </c>
+      <c r="P18">
+        <v>2.9</v>
+      </c>
+      <c r="Q18">
+        <v>0.1131</v>
+      </c>
+      <c r="R18" t="s">
         <v>42</v>
       </c>
-      <c r="C18" t="s">
+      <c r="S18" t="s">
         <v>48</v>
-      </c>
-      <c r="D18">
-        <v>44.61</v>
-      </c>
-      <c r="E18">
-        <v>4.37</v>
-      </c>
-      <c r="F18">
-        <v>14.41</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>10.6</v>
-      </c>
-      <c r="J18">
-        <v>0.17</v>
-      </c>
-      <c r="K18">
-        <v>7.69</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>11.55</v>
-      </c>
-      <c r="O18">
-        <v>3.93</v>
-      </c>
-      <c r="P18">
-        <v>1.74</v>
-      </c>
-      <c r="Q18">
-        <v>0.92</v>
-      </c>
-      <c r="R18">
-        <v>2.9</v>
-      </c>
-      <c r="S18">
-        <v>0.1131</v>
       </c>
       <c r="T18">
         <v>1500</v>

</xml_diff>

<commit_message>
Restructure files so that the entire library is not duplicated in the lib folder for pushing to pip.
</commit_message>
<xml_diff>
--- a/manuscript/testsave.xlsx
+++ b/manuscript/testsave.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="65">
   <si>
     <t>CITATION</t>
   </si>
@@ -695,7 +695,7 @@
         <v>0.4246947187776288</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>0.002873020370883501</v>
       </c>
       <c r="T2">
         <v>62.5</v>
@@ -1890,7 +1890,7 @@
         <v>0.4246947187776288</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>0.002873020370883501</v>
       </c>
       <c r="R2" t="s">
         <v>37</v>
@@ -3394,7 +3394,7 @@
         <v>0.4246947187776288</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>0.002873020370883501</v>
       </c>
       <c r="R2" t="s">
         <v>37</v>
@@ -3409,7 +3409,7 @@
         <v>1299.094712370722</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W2">
         <v>0</v>
@@ -3422,6 +3422,9 @@
       </c>
       <c r="Z2" t="s">
         <v>56</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -4847,7 +4850,7 @@
         <v>0.4246947187776288</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>0.002873020370883501</v>
       </c>
       <c r="R2" t="s">
         <v>37</v>
@@ -4862,10 +4865,10 @@
         <v>1299.094712370722</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <v>0.586163616167993</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>0.413836383832007</v>
       </c>
       <c r="X2" t="s">
         <v>56</v>
@@ -6201,7 +6204,7 @@
         <v>0.4246947187776288</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>0.002873020370883501</v>
       </c>
       <c r="R2" t="s">
         <v>37</v>
@@ -6216,22 +6219,22 @@
         <v>1299.094712370722</v>
       </c>
       <c r="V2">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="W2">
         <v>925</v>
       </c>
       <c r="X2">
-        <v>1</v>
+        <v>0.469913142701622</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>0.530086857298378</v>
       </c>
       <c r="Z2">
-        <v>0.0689581288685595</v>
+        <v>0.000835660852316802</v>
       </c>
       <c r="AA2">
-        <v>0.06895812886855952</v>
+        <v>0.0008356608523168019</v>
       </c>
       <c r="AB2" t="s">
         <v>56</v>
@@ -7759,7 +7762,7 @@
         <v>0.4246947187776288</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>0.002873020370883501</v>
       </c>
       <c r="R2" t="s">
         <v>37</v>
@@ -7774,19 +7777,19 @@
         <v>1299.094712370722</v>
       </c>
       <c r="V2">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="W2">
-        <v>1</v>
+        <v>0.493184396494459</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>0.506815603505541</v>
       </c>
       <c r="Y2">
-        <v>0.0777634607490745</v>
+        <v>0.000609818058643469</v>
       </c>
       <c r="Z2">
-        <v>0.07776346074907453</v>
+        <v>0.0006098180586434687</v>
       </c>
       <c r="AA2" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
Changes to manuscript during proof stage.
</commit_message>
<xml_diff>
--- a/manuscript/testsave.xlsx
+++ b/manuscript/testsave.xlsx
@@ -6317,10 +6317,10 @@
         <v>0.7844709533493121</v>
       </c>
       <c r="Z3">
-        <v>3.75646222415579e-05</v>
+        <v>3.75646222415579E-05</v>
       </c>
       <c r="AA3">
-        <v>3.756462224155789e-05</v>
+        <v>3.756462224155789E-05</v>
       </c>
       <c r="AB3" t="s">
         <v>56</v>
@@ -7435,10 +7435,10 @@
         <v>0.768292178983787</v>
       </c>
       <c r="Z16">
-        <v>9.309173835698601e-05</v>
+        <v>9.309173835698601E-05</v>
       </c>
       <c r="AA16">
-        <v>9.309173835698606e-05</v>
+        <v>9.309173835698606E-05</v>
       </c>
       <c r="AB16" t="s">
         <v>56</v>

</xml_diff>